<commit_message>
Added JiraUtil and Reporting
</commit_message>
<xml_diff>
--- a/AutomationRobo/Data/Config.xlsx
+++ b/AutomationRobo/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationRobo\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitin.verma\Desktop\UIPath-Project\AutomationRobo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C5F30B-949D-44F8-9943-9D38BE40D034}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC012D37-6DB9-49EA-A43C-75C83C355FFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -430,16 +430,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="68.5546875" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1491,16 +1491,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>